<commit_message>
added color style support
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingBase.xlsx
+++ b/src/test/resources/TestingBase.xlsx
@@ -119,7 +119,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -137,6 +137,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,7 +224,7 @@
   <dimension ref="C3:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,7 +297,9 @@
       <c r="C7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
   </sheetData>

</xml_diff>